<commit_message>
Updated with constellation data
</commit_message>
<xml_diff>
--- a/cat/CGs.xlsx
+++ b/cat/CGs.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mj\src\python\astropy-workbench\cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B15C8143-3DC3-47A4-88F3-76743B157052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD0C163-A189-48F9-BBBB-3515412BE14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="16875" xr2:uid="{41EC3EAF-2F58-4446-9732-1F41D77C4B14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{41EC3EAF-2F58-4446-9732-1F41D77C4B14}"/>
   </bookViews>
   <sheets>
     <sheet name="CGs" sheetId="1" r:id="rId1"/>
+    <sheet name="CGs with constellation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="145">
   <si>
     <t>Names</t>
   </si>
@@ -401,6 +415,60 @@
   </si>
   <si>
     <t>CG Name</t>
+  </si>
+  <si>
+    <t>Sagittarius</t>
+  </si>
+  <si>
+    <t>Sgr</t>
+  </si>
+  <si>
+    <t>Cassiopeia</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>Puppis</t>
+  </si>
+  <si>
+    <t>Pup</t>
+  </si>
+  <si>
+    <t>Pyxis</t>
+  </si>
+  <si>
+    <t>Pyx</t>
+  </si>
+  <si>
+    <t>Carina</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Vela</t>
+  </si>
+  <si>
+    <t>Vel</t>
+  </si>
+  <si>
+    <t>Musca</t>
+  </si>
+  <si>
+    <t>Mus</t>
+  </si>
+  <si>
+    <t>Centaurus</t>
+  </si>
+  <si>
+    <t>Cen</t>
+  </si>
+  <si>
+    <t>Constellation</t>
+  </si>
+  <si>
+    <t>Constellation short</t>
   </si>
 </sst>
 </file>
@@ -890,11 +958,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1270,9 +1339,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E8EA9D-923E-41A6-86A4-12CC5E50B9AA}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1911,10 +1980,918 @@
         <v>50</v>
       </c>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D42">
     <sortCondition ref="A2:A42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEC33E-12C3-4F97-ABCA-168043A5705B}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IFERROR(MID(A2,1,FIND(" /", A2)),A2)</f>
+        <v xml:space="preserve">CG1 DN </v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B42" si="0">IFERROR(MID(A3,1,FIND(" /", A3)),A3)</f>
+        <v xml:space="preserve">CG2 DN </v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG3 DN </v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG4 DN </v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG5 DN </v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG6 DN </v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG7 DN </v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>CG7S DN</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG8 DN </v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG9 DN </v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG10 DN </v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG11 DN </v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG12 DN </v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG13 DN </v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG14 DN </v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG15 DN </v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG16 DN </v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG17 DN </v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG18 DN </v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG19 DN </v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG20 DN </v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG21 DN </v>
+      </c>
+      <c r="C23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG22 DN </v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG24 DN </v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG25 DN </v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG26 DN </v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG27 DN </v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG28 DN </v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG29 DN </v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG30 DN </v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG31 DN </v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG31A DN </v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG31B DN </v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG31C DN </v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG31D DN </v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG32 DN </v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG33 DN </v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG34 DN </v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">CG36 DN </v>
+      </c>
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>CG37 DN</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>CG38 DN</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
+    <sortCondition ref="A2:A42"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>